<commit_message>
update fields on json - 2.1.
</commit_message>
<xml_diff>
--- a/2.1. Registro y actualizacion de articulos/campos_unibell.xlsx
+++ b/2.1. Registro y actualizacion de articulos/campos_unibell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffc\Desktop\Dev_EVOL\Unibell\2.1. Registro y actualizacion de articulos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRAINING1\Desktop\EVOL - FIELDS\Intergración WMS\2.1. Registro y actualizacion de articulos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E992A42-CE05-4CD2-A02C-F2B087A2EA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD96B2A-28F0-4773-8C70-8D8F6C8B57E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{C9569CFA-CC0E-4510-B81D-A697A083C165}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C9569CFA-CC0E-4510-B81D-A697A083C165}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="191">
   <si>
     <t>INTERNAL_ID</t>
   </si>
@@ -599,6 +599,18 @@
   <si>
     <t>Para los artículos
  de tipo ensamblaje</t>
+  </si>
+  <si>
+    <t>Solicitud de campo</t>
+  </si>
+  <si>
+    <t>custitem_pe_inventory_catalog</t>
+  </si>
+  <si>
+    <t>autoreorderpoint</t>
+  </si>
+  <si>
+    <t>autoleadtime</t>
   </si>
 </sst>
 </file>
@@ -737,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -768,6 +780,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1106,17 +1124,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17810B3-4352-4FF3-9BFA-B36E540C90AF}">
   <dimension ref="B2:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1124,7 +1142,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1132,172 +1150,172 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
@@ -1311,18 +1329,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB49CB3-079C-437B-AE71-A964E488500E}">
   <dimension ref="B2:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="58.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="58.7265625" customWidth="1"/>
+    <col min="4" max="4" width="45.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C2" s="8" t="s">
         <v>42</v>
       </c>
@@ -1330,7 +1348,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
         <v>37</v>
       </c>
@@ -1338,7 +1356,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4" s="5" t="s">
         <v>39</v>
       </c>
@@ -1346,7 +1364,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>43</v>
       </c>
@@ -1354,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" s="5" t="s">
         <v>44</v>
       </c>
@@ -1362,7 +1380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C7" s="5" t="s">
         <v>46</v>
       </c>
@@ -1370,7 +1388,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C8" s="5" t="s">
         <v>47</v>
       </c>
@@ -1378,7 +1396,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C9" s="5" t="s">
         <v>49</v>
       </c>
@@ -1386,7 +1404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C10" s="5" t="s">
         <v>50</v>
       </c>
@@ -1394,7 +1412,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
@@ -1402,7 +1420,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
         <v>54</v>
       </c>
@@ -1410,7 +1428,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
         <v>55</v>
       </c>
@@ -1418,7 +1436,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
         <v>56</v>
       </c>
@@ -1426,7 +1444,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
         <v>57</v>
       </c>
@@ -1434,7 +1452,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C16" s="5" t="s">
         <v>62</v>
       </c>
@@ -1442,7 +1460,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="5" t="s">
         <v>63</v>
       </c>
@@ -1450,7 +1468,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="5" t="s">
         <v>64</v>
       </c>
@@ -1458,7 +1476,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="5" t="s">
         <v>65</v>
       </c>
@@ -1466,7 +1484,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="5" t="s">
         <v>66</v>
       </c>
@@ -1474,7 +1492,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="5" t="s">
         <v>67</v>
       </c>
@@ -1482,7 +1500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="5" t="s">
         <v>73</v>
       </c>
@@ -1490,7 +1508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="5" t="s">
         <v>74</v>
       </c>
@@ -1498,7 +1516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="5" t="s">
         <v>75</v>
       </c>
@@ -1506,7 +1524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="5" t="s">
         <v>76</v>
       </c>
@@ -1514,7 +1532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="5" t="s">
         <v>77</v>
       </c>
@@ -1522,7 +1540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" s="5" t="s">
         <v>78</v>
       </c>
@@ -1530,7 +1548,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C28" s="5" t="s">
         <v>79</v>
       </c>
@@ -1538,7 +1556,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C29" s="5" t="s">
         <v>80</v>
       </c>
@@ -1546,7 +1564,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C30" s="5" t="s">
         <v>81</v>
       </c>
@@ -1554,7 +1572,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C31" s="5" t="s">
         <v>82</v>
       </c>
@@ -1562,7 +1580,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C32" s="5" t="s">
         <v>83</v>
       </c>
@@ -1570,7 +1588,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C33" s="5" t="s">
         <v>90</v>
       </c>
@@ -1578,7 +1596,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C34" s="6" t="s">
         <v>91</v>
       </c>
@@ -1586,7 +1604,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C35" s="5" t="s">
         <v>92</v>
       </c>
@@ -1594,7 +1612,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C36" s="5" t="s">
         <v>93</v>
       </c>
@@ -1602,7 +1620,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C37" s="5" t="s">
         <v>94</v>
       </c>
@@ -1610,7 +1628,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C38" s="5" t="s">
         <v>95</v>
       </c>
@@ -1618,7 +1636,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C39" s="5" t="s">
         <v>96</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C40" s="5" t="s">
         <v>97</v>
       </c>
@@ -1634,7 +1652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C41" s="5" t="s">
         <v>98</v>
       </c>
@@ -1642,7 +1660,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C42" s="5" t="s">
         <v>99</v>
       </c>
@@ -1650,7 +1668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C43" s="5" t="s">
         <v>100</v>
       </c>
@@ -1658,7 +1676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C44" s="5" t="s">
         <v>101</v>
       </c>
@@ -1666,7 +1684,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C45" s="5" t="s">
         <v>102</v>
       </c>
@@ -1674,7 +1692,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C46" s="5" t="s">
         <v>103</v>
       </c>
@@ -1682,7 +1700,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C47" s="5" t="s">
         <v>104</v>
       </c>
@@ -1690,7 +1708,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C48" s="5" t="s">
         <v>105</v>
       </c>
@@ -1698,7 +1716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C49" s="5" t="s">
         <v>106</v>
       </c>
@@ -1706,7 +1724,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C50" s="5" t="s">
         <v>107</v>
       </c>
@@ -1714,7 +1732,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C51" s="5" t="s">
         <v>108</v>
       </c>
@@ -1722,7 +1740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C52" s="5" t="s">
         <v>109</v>
       </c>
@@ -1730,7 +1748,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C53" s="5" t="s">
         <v>110</v>
       </c>
@@ -1738,7 +1756,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C54" s="5" t="s">
         <v>111</v>
       </c>
@@ -1746,7 +1764,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C55" s="5" t="s">
         <v>127</v>
       </c>
@@ -1754,7 +1772,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C56" s="7" t="s">
         <v>128</v>
       </c>
@@ -1762,245 +1780,251 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C57" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D57" s="5"/>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C58" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D58" s="5"/>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C59" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C60" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="12" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C61" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C62" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="12" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C63" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C64" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C65" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="12" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C66" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="12" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C67" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C68" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C69" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="12" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C70" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B71" s="9" t="s">
         <v>186</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="10"/>
       <c r="C72" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="13" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B73" s="10"/>
       <c r="C73" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="11"/>
       <c r="C74" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="13" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C75" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C76" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C77" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C78" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C79" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C80" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D80" s="12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C81" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C82" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C83" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="12" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C84" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C85" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C86" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D86" s="5"/>
+      <c r="D86" s="12" t="s">
+        <v>187</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add jerarqui field - 2.1.
</commit_message>
<xml_diff>
--- a/2.1. Registro y actualizacion de articulos/campos_unibell.xlsx
+++ b/2.1. Registro y actualizacion de articulos/campos_unibell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRAINING1\Desktop\EVOL - FIELDS\Intergración WMS\2.1. Registro y actualizacion de articulos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD96B2A-28F0-4773-8C70-8D8F6C8B57E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902E12B3-B718-43DC-B10C-FA178889490F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C9569CFA-CC0E-4510-B81D-A697A083C165}"/>
   </bookViews>
@@ -617,7 +617,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,6 +647,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -749,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -786,6 +793,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1329,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB49CB3-079C-437B-AE71-A964E488500E}">
   <dimension ref="B2:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1950,7 +1960,7 @@
       <c r="C77" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="14" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1958,7 +1968,7 @@
       <c r="C78" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="14" t="s">
         <v>188</v>
       </c>
     </row>
@@ -1998,7 +2008,7 @@
       <c r="C83" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D83" s="14" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2031,5 +2041,6 @@
     <mergeCell ref="B71:B74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>